<commit_message>
Began edits on Test layout with color coded tests
</commit_message>
<xml_diff>
--- a/room_and_test_layout.xlsx
+++ b/room_and_test_layout.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hayden/Documents/Java/ClueGameExp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="19480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="31">
   <si>
     <t>X</t>
   </si>
@@ -88,6 +98,27 @@
   </si>
   <si>
     <t>DL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Doors: </t>
+  </si>
+  <si>
+    <t>White: Door Direction Tests</t>
+  </si>
+  <si>
+    <t>OrangeL Adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: Adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Light Purple: walkway test scenarios</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -153,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -166,6 +197,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -228,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="3.7109375" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="3.28515625" style="1"/>
+    <col min="1" max="26" width="3.6640625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="3.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -564,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -644,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -724,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -804,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -884,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -964,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1124,7 +1158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1204,7 +1238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1364,7 +1398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1444,7 +1478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1524,7 +1558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1604,7 +1638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1684,7 +1718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1764,7 +1798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1844,7 +1878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1924,7 +1958,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2004,7 +2038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2084,7 +2118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2164,7 +2198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2241,7 +2275,128 @@
         <v>24</v>
       </c>
     </row>
+    <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A29:L29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2253,7 +2408,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2265,7 +2420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>